<commit_message>
if co-existence is false then MISYS and KONNECT will run else all 3 MISYS, TRANSACT and KONNECT will run
</commit_message>
<xml_diff>
--- a/Test Cases MW APIs Only Aasan Account.xlsx
+++ b/Test Cases MW APIs Only Aasan Account.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\services\Coexistence\OnlyAasanAccount\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41FFB7E-EC17-4D53-9CD5-4AAFEA3753AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{862CEDB6-9A87-4FD3-92DC-4A7237F60238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CB6F9772-5A0C-497F-B682-E471106FD732}"/>
   </bookViews>
@@ -1312,7 +1312,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added 3 new channels, MYSIS, KONNECT, TRANSACT
</commit_message>
<xml_diff>
--- a/Test Cases MW APIs Only Aasan Account.xlsx
+++ b/Test Cases MW APIs Only Aasan Account.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\services\Coexistence\OnlyAasanAccount\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{862CEDB6-9A87-4FD3-92DC-4A7237F60238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D615C37-69F7-4DC5-8D1E-6F5DFE9B59E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CB6F9772-5A0C-497F-B682-E471106FD732}"/>
   </bookViews>
@@ -988,10 +988,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1311,8 +1311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACDD609F-8BE0-421C-A3F9-F52953AAA3DE}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1516,13 +1516,13 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="240" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>